<commit_message>
processed datasets and subset datasets into area of residences,  created combined attribute file
</commit_message>
<xml_diff>
--- a/Data/AgeGroup_2020_Cleaned.xlsx
+++ b/Data/AgeGroup_2020_Cleaned.xlsx
@@ -1,15 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yi Zhen\Documents\GitHub\BT4015\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00228E16-67D5-47BA-AAC3-537EE2D59D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -190,8 +207,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +271,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -300,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,9 +357,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,6 +409,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,14 +602,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -600,7 +667,7 @@
         <v>899010</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -626,7 +693,7 @@
         <v>47950</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -652,7 +719,7 @@
         <v>75230</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -678,7 +745,7 @@
         <v>23170</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -704,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -730,7 +797,7 @@
         <v>33420</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -756,7 +823,7 @@
         <v>44420</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -782,7 +849,7 @@
         <v>27890</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -808,7 +875,7 @@
         <v>18040</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -834,7 +901,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -860,7 +927,7 @@
         <v>32830</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -886,7 +953,7 @@
         <v>24700</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -912,7 +979,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -938,7 +1005,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -964,7 +1031,7 @@
         <v>55530</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -990,7 +1057,7 @@
         <v>21640</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1016,7 +1083,7 @@
         <v>51550</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1042,7 +1109,7 @@
         <v>29050</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1068,7 +1135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1094,7 +1161,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1120,7 +1187,7 @@
         <v>12190</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1146,7 +1213,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1172,7 +1239,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1198,7 +1265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1224,7 +1291,7 @@
         <v>11750</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1250,7 +1317,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1276,7 +1343,7 @@
         <v>6140</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1302,7 +1369,7 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1328,7 +1395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1354,7 +1421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1380,7 +1447,7 @@
         <v>19840</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1406,7 +1473,7 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1432,7 +1499,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1458,7 +1525,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1484,7 +1551,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1510,7 +1577,7 @@
         <v>14700</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1536,7 +1603,7 @@
         <v>37870</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1562,7 +1629,7 @@
         <v>32590</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1655,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1614,7 +1681,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1640,7 +1707,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1666,7 +1733,7 @@
         <v>59620</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1692,7 +1759,7 @@
         <v>4460</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1718,7 +1785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1744,7 +1811,7 @@
         <v>34950</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1770,7 +1837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1796,7 +1863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1822,7 +1889,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1848,7 +1915,7 @@
         <v>41480</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>56</v>
       </c>

</xml_diff>